<commit_message>
Update reading Inventory file
</commit_message>
<xml_diff>
--- a/Sufficient data WITH_PO/forecast_summary_B083NMK4BB_WITH_PO.xlsx
+++ b/Sufficient data WITH_PO/forecast_summary_B083NMK4BB_WITH_PO.xlsx
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>1.18</v>
+        <v>1.13</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>1.1</v>
+        <v>0.85</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.93</v>
+        <v>1.16</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>1.09</v>
+        <v>0.8</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0.86</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.83</v>
+        <v>1.1</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>1.18</v>
+        <v>0.96</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.96</v>
+        <v>1.2</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>1.06</v>
+        <v>1.15</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>0.89</v>
+        <v>1.03</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>0.8</v>
+        <v>1.13</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>1.16</v>
+        <v>1.05</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>

</xml_diff>